<commit_message>
Scaling (with calibration) and triggering working
</commit_message>
<xml_diff>
--- a/VM registers.xlsx
+++ b/VM registers.xlsx
@@ -1155,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1356,11 +1356,11 @@
         <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>"vrTriggerIntro": (0x32, 'U24', "Edge trigger intro filter counter (samples/2)"),</v>
+        <v>"vrTriggerIntro": (0x32, 'U16', "Edge trigger intro filter counter (samples/2)"),</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20" x14ac:dyDescent="0.25">

</xml_diff>